<commit_message>
add filters in gos_zakupki_parser.py
</commit_message>
<xml_diff>
--- a/zakupki_223.xlsx
+++ b/zakupki_223.xlsx
@@ -473,133 +473,133 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>№ 32515384384</t>
+          <t>№ 32515362809</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "ИНТЕЛЛЕКТУАЛЬНЫЕ КОММУНАЛЬНЫЕ СИСТЕМЫ КОРСАКОВ"</t>
+          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "УЧЕБНО-ОПЫТНЫЙ МОЛОЧНЫЙ ЗАВОД" ВОЛОГОДСКОЙ ГОСУДАРСТВЕННОЙ МОЛОЧНОХОЗЯЙСТВЕННОЙ АКАДЕМИИ ИМЕНИ Н.В. ВЕРЕЩАГИНА"</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Поставка шин для автомобильного транспорта ООО «ИКС-Корсаков»</t>
+          <t>Поставка защитной одежды (перчатки, бахилы, маски, халаты, шапочки-береты, фартуки)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2 782 231,67 ₽</t>
+          <t>1 900 070,00 ₽</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
+          <t>31.10.2025, 10.11.2025, 19.11.2025</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>223-ФЗ Конкурс в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Прочие</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995943</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18997432</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>№ 32515383544</t>
+          <t>№ 32515336859</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "ЭНЕРГОЦЕНТР БИЛИБИНО"</t>
+          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "УЧЕБНО-ОПЫТНЫЙ МОЛОЧНЫЙ ЗАВОД" ВОЛОГОДСКОЙ ГОСУДАРСТВЕННОЙ МОЛОЧНОХОЗЯЙСТВЕННОЙ АКАДЕМИИ ИМЕНИ Н.В. ВЕРЕЩАГИНА"</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Услуги по физической охране объекта «Энергоцентр Билибино с внеплощадочной инфраструктурой», расположенного по адресу: г. Билибино.</t>
+          <t>Поставка сухих питательных сред</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>8 278 200,00 ₽</t>
+          <t>3 000 000,00 ₽</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 25.11.2025</t>
+          <t>24.10.2025, 10.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994798</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18997315</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>№ 32515363856</t>
+          <t>№ 32515380971</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ ДОШКОЛЬНОЕ ОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ ЦЕНТР РАЗВИТИЯ РЕБЕНКА - ДЕТСКИЙ САД № 14 "РЯБИНКА" Г. ЮЖНО-САХАЛИНСКА</t>
+          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ ФИЗИЧЕСКОЙ КУЛЬТУРЫ И СПОРТА ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР СПОРТИВНОЙ ПОДГОТОВКИ"</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Оказание услуг по охране объекта и имущества, а также обеспечение внутриобъектового и пропускного режима на объекте, в отношении которого установлены обязательные для выполнения требования к антитеррористической защищенности объекта</t>
+          <t>Поставка сувенирной продукции (наградная фигура)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>6 132 000,00 ₽</t>
+          <t>102 700,00 ₽</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>01.11.2025, 10.11.2025, 15.11.2025</t>
+          <t>07.11.2025, 10.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>223-ФЗ Конкурс в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994845</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18997253</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>№ 32515383401</t>
+          <t>№ 32515385421</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ПУБЛИЧНОЕ АКЦИОНЕРНОЕ ОБЩЕСТВО ЭНЕРГЕТИКИ И ЭЛЕКТРИФИКАЦИИ "МАГАДАНЭНЕРГО"</t>
+          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "УЧЕБНО-ОПЫТНЫЙ МОЛОЧНЫЙ ЗАВОД" ВОЛОГОДСКОЙ ГОСУДАРСТВЕННОЙ МОЛОЧНОХОЗЯЙСТВЕННОЙ АКАДЕМИИ ИМЕНИ Н.В. ВЕРЕЩАГИНА"</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ОКПД 2 28.23.2 Поставка расходных материалов и запасных частей для копировальной и оргтехники для нужд ПАО "Магаданэнерго" (Лот № 23501-ЭКСП ПРОД-2025-МЭ)</t>
+          <t>Поставка фильтрующих элементов (картриджей) для фильтров тонкой очистки молока</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>5 645 255,27 ₽</t>
+          <t>444 400,00 ₽</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -609,72 +609,76 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994788</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18997174</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>№ 32515385222</t>
+          <t>№ 32515385341</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "СЕВЕРСКИЙ ВОДОКАНАЛ"</t>
+          <t>МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ ГОРОДА ЧЕРЕПОВЦА "ТЕПЛОЭНЕРГИЯ"</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Поставка новогоднего освещения и украшений для оформления уличной ели</t>
+          <t>Выполнение работ по очистке кровли от снега, наледи и сосулек на многоквартирных жилых домах МУП «Теплоэнергия»</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>256 100,00 ₽</t>
+          <t>1 197 666,67 ₽</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>10.11.2025, 10.11.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995452</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18997109</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>№ 32515383289</t>
+          <t>№ 32515385231</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ПУБЛИЧНОЕ АКЦИОНЕРНОЕ ОБЩЕСТВО ЭНЕРГЕТИКИ И ЭЛЕКТРИФИКАЦИИ "САХАЛИНЭНЕРГО"</t>
+          <t>МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ ГОРОДА ЧЕРЕПОВЦА "ТЕПЛОЭНЕРГИЯ"</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>№ 1701-РЕМ ПРОД-2026-СЭ: «ОКПД2 29.10.12.000. Поставка контрактных двигателей импортного производства для нужд ОП «Южно-Сахалинская ТЭЦ-1»; № 1702-РЕМ ПРОД-2026-СЭ «ОКПД2 29.10.12.000. Поставка двигателя внутреннего сгорания отечественного производства для нужд ОП «Южно-Сахалинская ТЭЦ-1»</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
+          <t>Оказание услуг по удалению насаждений (деревья, кустарники) для оборудования запретной зоны на территории объектов МУП «Теплоэнергия»</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1 229 333,33 ₽</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 26.11.2025</t>
+          <t>10.11.2025, 10.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -684,29 +688,29 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994648</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996986</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>№ 32515385065</t>
+          <t>№ 32515385074</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "КРАСНОЯРСКОЕ ПАССАЖИРСКОЕ АВТОТРАНСПОРТНОЕ ПРЕДПРИЯТИЕ № 5"</t>
+          <t>МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ "ЧЕРЕПОВЕЦКАЯ АВТОКОЛОННА № 1456"</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>выполнение работ по разработке проектно-сметной документации на «Капитальный ремонт инженерных сетей нежилого здания гаража для организации мероприятий по расположению и ремонту транспортных средств, работающих на сжиженном природном газе, расположенного по адресу: г. Красноярск, ул. Калинина, д.84, стр.6»</t>
+          <t>Поставка ГБЦ</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>18 001 666,67 ₽</t>
+          <t>353 212,00 ₽</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -716,39 +720,39 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Прочие</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996698</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996808</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>№ 32515383505</t>
+          <t>№ 32515384987</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "ВОЕНТОРГ-ВОСТОК"</t>
+          <t>МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ ГОРОДА ЧЕРЕПОВЦА "ТЕПЛОЭНЕРГИЯ"</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Комплекс работ по ремонту кровли объекта, расположенного по адресу: Красноярский край, ЗАТО Солнечный, ул. Неделина, 18В</t>
+          <t>Поставка датчика пламени и реле давления</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>403 114,69 ₽</t>
+          <t>42 525,00 ₽</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 14.11.2025</t>
+          <t>10.11.2025, 10.11.2025, 13.11.2025</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -758,66 +762,66 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994890</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996704</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>№ 32515383897</t>
+          <t>№ 32515384818</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ФЕДЕРАЛЬНОЕ ГОСУДАРСТВЕННОЕ БЮДЖЕТНОЕ ОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ ВЫСШЕГО ОБРАЗОВАНИЯ "АРКТИЧЕСКИЙ ГОСУДАРСТВЕННЫЙ ИНСТИТУТ КУЛЬТУРЫ И ИСКУССТВ"</t>
+          <t>МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ ГОРОДА ЧЕРЕПОВЦА "ТЕПЛОЭНЕРГИЯ"</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Услуги проживания в гостинице</t>
+          <t>Поставка регулятора-стабилизатора давления газа</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>325 000,00 ₽</t>
+          <t>44 754,80 ₽</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>10.11.2025, 10.11.2025, 13.11.2025</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>223-ФЗ Закупка у единственного поставщика (подрядчика, исполнителя)</t>
+          <t>223-ФЗ Прочие</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995415</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996483</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>№ 32515384924</t>
+          <t>№ 32515384814</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "ГАРАНТИЙНЫЙ ФОНД ТОМСКОЙ ОБЛАСТИ"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ "ЦЕНТР МУНИЦИПАЛЬНЫХ ИНФОРМАЦИОННЫХ РЕСУРСОВ И ТЕХНОЛОГИЙ"</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Выполнение работ по изготовлению полиграфической продукции</t>
+          <t>Поставка системного блока</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>193 160,17 ₽</t>
+          <t>40 900,00 ₽</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -832,66 +836,66 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996368</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996467</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>№ 32515383493</t>
+          <t>№ 32515384766</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>КРАЕВОЕ ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ ДОПОЛНИТЕЛЬНОГО ОБРАЗОВАНИЯ "СПОРТИВНАЯ ШКОЛА ОЛИМПИЙСКОГО РЕЗЕРВА "ЕРОФЕЙ"</t>
+          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "ШЕКСНА-ТЕПЛОСЕТЬ"</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Поставка и монтаж системы видеонаблюдения с функцией видеоаналитики и предоставлением доступа в облачную платформу видеонаблюдения, интегрированную с сервисом, предназначенным для анализа и измерения загруженности объектов спорта на территории Хабаровского края и обеспечивающим обмен данными с автоматизированной системой управления в сфере физической культуры и спорта, используемой в Хабаровском крае для нужд КГАУ ДО СШОР «Ерофей»</t>
+          <t>Поставка канцелярских товаров</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>5 400 729,33 ₽</t>
+          <t>38 507,40 ₽</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
+          <t>10.11.2025, 10.11.2025</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Закупка у единственного поставщика (подрядчика, исполнителя)</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994908</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996428</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>№ 32515384849</t>
+          <t>№ 32515384752</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ ОБЩЕОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ НОВОСИБИРСКОГО РАЙОНА НОВОСИБИРСКОЙ ОБЛАСТИ "ГИМНАЗИЯ "КРАСНООБСКАЯ"</t>
+          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "ШЕКСНА-ТЕПЛОСЕТЬ"</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Поставка офисной бумаги для обеспечения жизнедеятельности МАОУ «Гимназия «Краснообская»</t>
+          <t>Поставка офисной бумаги для печати</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>160 000,00 ₽</t>
+          <t>20 040,00 ₽</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -906,103 +910,103 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996497</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996400</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>№ 32515384845</t>
+          <t>№ 32515380744</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ НОВОСИБИРСКОЙ ОБЛАСТИ "НОВОСИБИРСКИЙ ОБЛАСТНОЙ КЛИНИЧЕСКИЙ НАРКОЛОГИЧЕСКИЙ ДИСПАНСЕР"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ "ЦЕНТР СОЦИАЛЬНОГО ПИТАНИЯ"</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Поставка лекарственных препаратов для медицинского применения</t>
+          <t>Поставка продуктов питания для нужд МАУ "Центр социального питания" (лот 3)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>81 195,60 ₽</t>
+          <t>31 912 745,00 ₽</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 17.11.2025</t>
+          <t>07.11.2025, 10.11.2025, 24.11.2025</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996521</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995712</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>№ 32515384825</t>
+          <t>№ 32515383475</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ ПРОФЕССИОНАЛЬНОЕ ОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ НОВОСИБИРСКОЙ ОБЛАСТИ "НОВОСИБИРСКИЙ АРХИТЕКТУРНО-СТРОИТЕЛЬНЫЙ КОЛЛЕДЖ"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ ОБЩЕОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ "НАЧАЛЬНАЯ ШКОЛА - ДЕТСКИЙ САД № 98 "ХРУСТАЛИК"</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Поставка продуктов питания (бакалея)</t>
+          <t>Ремонт МАОУ «Начальная школа - детский сад № 98 «Хрусталик» по адресу: г. Вологда, ул. Ярославская, д. 24а (замена оконных блоков)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>256 636,92 ₽</t>
+          <t>1 767 656,21 ₽</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 13.11.2025</t>
+          <t>10.11.2025, 10.11.2025</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Закупка у единственного поставщика (подрядчика, исполнителя)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996505</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18989398</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>№ 32515383028</t>
+          <t>№ 32515383262</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ПУБЛИЧНОЕ АКЦИОНЕРНОЕ ОБЩЕСТВО ЭНЕРГЕТИКИ И ЭЛЕКТРИФИКАЦИИ "САХАЛИНЭНЕРГО"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ "ЦЕНТР СОЦИАЛЬНОГО ПИТАНИЯ"</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Лот № 0067-РЕМ ПРОД-2026-СЭ. Право заключения договора на поставку асботехнических материалов для герметизации различных соединений для нужд филиала "Распределительные сети", ОП "Южно-Сахалинская ТЭЦ-1", ОП «Сахалинская ГРЭС»</t>
+          <t>Поставка продуктов питания для нужд МАУ "Центр социального питания" (лот 6)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>5 830 419,88 ₽</t>
+          <t>4 717 000,00 ₽</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1012,34 +1016,34 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос предложений в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994311</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994617</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>№ 32515384780</t>
+          <t>№ 32515383098</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ ОБЩЕОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ НОВОСИБИРСКОГО РАЙОНА НОВОСИБИРСКОЙ ОБЛАСТИ "ГИМНАЗИЯ "КРАСНООБСКАЯ"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ "ЦЕНТР МУНИЦИПАЛЬНЫХ ИНФОРМАЦИОННЫХ РЕСУРСОВ И ТЕХНОЛОГИЙ"</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Поставка диванов для обеспечения жизнедеятельности МАОУ «Гимназия «Краснообская»</t>
+          <t>Услуги по установке, тестированию, сопровождению программ для ЭВМ системы "1С:Предприятие" и баз данных, включая базы данных 1С:ИТС</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>250 000,00 ₽</t>
+          <t>17 115,00 ₽</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1049,224 +1053,224 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>223-ФЗ Закупка у единственного поставщика (подрядчика, исполнителя)</t>
+          <t>223-ФЗ Прочие</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996409</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994396</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>№ 32515384731</t>
+          <t>№ 32515382715</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ОБЛАСТНОЕ ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ "ТОМСКИЙ ФТИЗИОПУЛЬМОНОЛОГИЧЕСКИЙ МЕДИЦИНСКИЙ ЦЕНТР"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ "ЦЕНТР СОЦИАЛЬНОГО ПИТАНИЯ"</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Поставка нефтепродуктов через АЗС (АЗК) по пластиковым (топливным) картам на 2026 год для автомобилей ОГАУЗ «ТФМЦ»</t>
+          <t>Поставка продуктов питания для нужд МАУ "Центр социального питания" (лот 5)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5 844 240,00 ₽</t>
+          <t>9 775 000,00 ₽</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 27.11.2025</t>
+          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996343</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18993825</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>№ 32515383719</t>
+          <t>№ 32515382408</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ ДОПОЛНИТЕЛЬНОГО ПРОФЕССИОНАЛЬНОГО ОБРАЗОВАНИЯ "ИНСТИТУТ НОВЫХ ТЕХНОЛОГИЙ РЕСПУБЛИКИ САХА (ЯКУТИЯ)"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ "ЦЕНТР СОЦИАЛЬНОГО ПИТАНИЯ"</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Оказание платных медицинских услуг</t>
+          <t>Поставка продуктов питания для нужд МАУ "Центр социального питания" (лот 4)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>193 980,00 ₽</t>
+          <t>6 933 200,00 ₽</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>223-ФЗ Закупка у единственного поставщика (подрядчика, исполнителя)</t>
+          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995176</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18993397</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>№ 32515385187</t>
+          <t>№ 32515382115</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ ДОШКОЛЬНОЕ ОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ ГОРОДА НОВОСИБИРСКА "ДЕТСКИЙ САД № 472 "ТИГРЁНОК"</t>
+          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "ЦЕНТР 112"</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Оказание услуг по охране помещений МАДОУ д/с 472</t>
+          <t>Оказание клининговых услуг</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>167 040,00 ₽</t>
+          <t>997 854,02 ₽</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>223-ФЗ Закупка у единственного поставщика (подрядчика, исполнителя)</t>
+          <t>223-ФЗ Прочие</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996910</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18992945</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>№ 32515382904</t>
+          <t>№ 32515381364</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ПУБЛИЧНОЕ АКЦИОНЕРНОЕ ОБЩЕСТВО ЭНЕРГЕТИКИ И ЭЛЕКТРИФИКАЦИИ "САХАЛИНЭНЕРГО"</t>
+          <t>ФЕДЕРАЛЬНОЕ ГОСУДАРСТВЕННОЕ БЮДЖЕТНОЕ ОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ ВЫСШЕГО ОБРАЗОВАНИЯ "ВОЛОГОДСКИЙ ГОСУДАРСТВЕННЫЙ УНИВЕРСИТЕТ"</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ОКПД2 28.29.12.110. Поставка фильтрующих элементов для водно-химической очистки воды для нужд ОП «Сахалинская ГРЭС» (Лот № 0174-ЭКСП ПРОД-2026-СЭ)</t>
+          <t>Микроавтобус</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>498 680,00 ₽</t>
+          <t>5 000 000,00 ₽</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 20.11.2025</t>
+          <t>09.11.2025, 10.11.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994137</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18992723</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>№ 32515245801</t>
+          <t>№ 32515380912</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ПУБЛИЧНОЕ АКЦИОНЕРНОЕ ОБЩЕСТВО ЭНЕРГЕТИКИ И ЭЛЕКТРИФИКАЦИИ "КАМЧАТСКЭНЕРГО"</t>
+          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ ДОПОЛНИТЕЛЬНОГО ОБРАЗОВАНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "СПОРТИВНАЯ ШКОЛА ОЛИМПИЙСКОГО РЕЗЕРВА "ВИТЯЗЬ"</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Право заключения договора по лоту: "ОКПД2 42.22.22 Выполнение строительно-монтажных работ и пусконаладочных работ по объекту «Сооружение ВЛ-35 кВ от ПС 110/35/10 кВ «Кавалерская» до Сооружения ДЭС-6 п. Усть-Большерецк, со строительством ВЛ-35 кВ и реконструкцией ПС 110/35/10 кВ «Кавалерская» и Сооружения ДЭС-6 п. Усть-Большерецк», в рамках инвестиционных проектов O_ЦЭС_509-4266, O_ЦЭС_509-4264, O_ЦЭС_509-4265, для нужд ПАО «Камчатскэнерго» (Лот № 96900-ТПИР ОБСЛ-2025-КамчЭн)"</t>
+          <t>Поставка стоек для хранения гимнастических палок</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>342 857 989,91 ₽</t>
+          <t>45 600,00 ₽</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>25.09.2025, 10.11.2025, 19.11.2025</t>
+          <t>07.11.2025, 07.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18993145</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18991194</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>№ 32515383306</t>
+          <t>№ 32515380685</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "УССУРИЙСКОЕ ПРЕДПРИЯТИЕ ТЕПЛОВЫХ СЕТЕЙ"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ "ЦЕНТР СОЦИАЛЬНОГО ПИТАНИЯ"</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>поставка новых годовых лицензий Платформа nanoCad (конфигурация Pro) для нужд АО «УПТС»</t>
+          <t>Закупка продуктов питания для нужд МАУ "Центр социального питания" (лот2)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1 048 333,33 ₽</t>
+          <t>15 543 080,85 ₽</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
+          <t>07.11.2025, 07.11.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1276,437 +1280,441 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994435</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18991098</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>№ 32515384115</t>
+          <t>№ 32515380667</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ ОБЩЕОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ "СРЕДНЯЯ ОБЩЕОБРАЗОВАТЕЛЬНАЯ ШКОЛА №54 Г.УЛАН-УДЭ"</t>
+          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ ДОПОЛНИТЕЛЬНОГО ОБРАЗОВАНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "СПОРТИВНАЯ ШКОЛА ОЛИМПИЙСКОГО РЕЗЕРВА "ВИТЯЗЬ"</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Оказание услуг по охране общественного порядка на объекте</t>
+          <t>Оказание услуг по техническому обслуживанию инженерных систем, внешних и внутренних систем электроснабжения, наружного и внутреннего освещения, оборудования в зданиях АУ ДО ВО "СШОР "Витязь"</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>292 800,00 ₽</t>
+          <t>1 950 000,00 ₽</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>07.11.2025, 07.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995676</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18990929</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>№ 32515385085</t>
+          <t>№ 32515380594</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>СПЕЦИАЛИЗИРОВАННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ ОМСКОЙ ОБЛАСТИ "МУРОМЦЕВСКИЙ ЛЕСХОЗ"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ "ЦЕНТР СОЦИАЛЬНОГО ПИТАНИЯ"</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Поставка вакуумной сушильной камеры для сушки древесины «Теравуд 18-6» для нужд специализированного автономного учреждения Омской области "Муромцевский лесхоз"</t>
+          <t>Поставка продуктов питания для нужд МАУ "Центр социального питания" (лот 1)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>5 715 000,00 ₽</t>
+          <t>11 675 000,00 ₽</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 12.11.2025</t>
+          <t>07.11.2025, 07.11.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996725</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18990966</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>№ 32515383987</t>
+          <t>№ 32515380509</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ОБЛАСТНОЕ ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ "ИРКУТСКАЯ ГОРОДСКАЯ КЛИНИЧЕСКАЯ БОЛЬНИЦА № 8"</t>
+          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "БЛАГОУСТРОЙСТВО"</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Поставка офисной бумаги</t>
+          <t>Выполнение работ капитального ремонта по замене выпусков канализации в многоквартирном доме по адресу: Вологодская область п. Шексна ул. Октябрьская 93</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>3 040 000,00 ₽</t>
+          <t>350 000,00 ₽</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 17.11.2025</t>
+          <t>07.11.2025, 07.11.2025, 10.11.2025</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Прочие</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995560</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18990782</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>№ 32515383189</t>
+          <t>№ 32515379931</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ПУБЛИЧНОЕ АКЦИОНЕРНОЕ ОБЩЕСТВО "ДАЛЬНЕВОСТОЧНАЯ ЭНЕРГЕТИЧЕСКАЯ КОМПАНИЯ"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ "ЦЕНТР МУНИЦИПАЛЬНЫХ ИНФОРМАЦИОННЫХ РЕСУРСОВ И ТЕХНОЛОГИЙ"</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ОКДП2 - 73.11.13.000 Услуги по проведению акций для клиентов филиалов ПАО "ДЭК" (лоты №12801 - №12806)</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr"/>
+          <t>Расходные материалы и запасные части для печатающей техники</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>278 712,00 ₽</t>
+        </is>
+      </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 17.11.2025</t>
+          <t>07.11.2025, 07.11.2025</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Прочие</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994491</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18990223</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>№ 32515383560</t>
+          <t>№ 32515379735</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "САХАТРАНСНЕФТЕГАЗ"</t>
+          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ ДОПОЛНИТЕЛЬНОГО ОБРАЗОВАНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "СПОРТИВНАЯ ШКОЛА ОЛИМПИЙСКОГО РЕЗЕРВА "ВИТЯЗЬ"</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Оказание услуг по сбору, транспортированию и обезвреживанию отходов III - IV классов опасности, образованных за 2 полугодие 2025 г. АО "Сахатранснефтегаз"</t>
+          <t>Оказание услуг по аренде и обслуживанию мобильных туалетных кабин (биотуалетов)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>572 388,00 ₽</t>
+          <t>114 000,00 ₽</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
+          <t>07.11.2025, 07.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994768</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18990063</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>№ 32515384963</t>
+          <t>№ 32515374710</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "МАГНИТ"</t>
+          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "ВОЛОГОДСКАЯ ОБЛАСТНАЯ ЭНЕРГЕТИЧЕСКАЯ КОМПАНИЯ"</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>поставка средств индивидуальной защиты (далее – услуга, предмет закупки).</t>
+          <t>Право заключения договора на оказание услуг по заправке и ремонту картриджей для нужд АО «Вологдаоблэнерго».</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>6 472 371,00 ₽</t>
+          <t>450 062,41 ₽</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
+          <t>06.11.2025, 07.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Запрос предложений в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996658</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18989822</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>№ 32515358898</t>
+          <t>№ 32515379407</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "УСТЬ-СРЕДНЕКАНГЭССТРОЙ"</t>
+          <t>МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ ГОРОДА ЧЕРЕПОВЦА "ВОДОКАНАЛ"</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ОКПД2 43.21.1 Выполнение электромонтажных работ в рамках работ по ремонту на оборудовании бункерно-деаэраторной этажерки Владивостокской ТЭЦ-2 (Лот № 0710-КС ДОХ-2025-УСГС)</t>
+          <t>Фильтровальный материал марки ОДМ-2Ф (опоки дробленые модифицированные)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2 633 495,32 ₽</t>
+          <t>5 032 747,52 ₽</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>31.10.2025, 10.11.2025, 14.11.2025</t>
+          <t>07.11.2025, 07.11.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Конкурс в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994367</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18989525</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>№ 32515384390</t>
+          <t>№ 32515378646</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "ГАРАНТИЙНЫЙ ФОНД ТОМСКОЙ ОБЛАСТИ"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ ОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ ДОПОЛНИТЕЛЬНОГО ОБРАЗОВАНИЯ "СПОРТИВНАЯ ШКОЛА ОЛИМПИЙСКОГО РЕЗЕРВА № 4"</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Поставка канцелярских товаров</t>
+          <t>Поставка строительных товаров</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>79 580,16 ₽</t>
+          <t>88 701,29 ₽</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>07.11.2025, 07.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995819</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18988636</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>№ 32515383831</t>
+          <t>№ 32515378465</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ ПРЕДПРИЯТИЕ РЕСПУБЛИКИ БУРЯТИЯ "БУРЯТ-ФАРМАЦИЯ"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ ОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ ДОПОЛНИТЕЛЬНОГО ОБРАЗОВАНИЯ "СПОРТИВНАЯ ШКОЛА ОЛИМПИЙСКОГО РЕЗЕРВА № 4"</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Поставка лекарственных препаратов</t>
+          <t>Поставка саней-волокуш</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>6 462 836,40 ₽</t>
+          <t>80 266,66 ₽</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 14.11.2025</t>
+          <t>07.11.2025, 07.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995359</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18988385</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>№ 32515385346</t>
+          <t>№ 32515378233</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ ЦЕНТР СПОРТИВНОЙ ПОДГОТОВКИ РЕСПУБЛИКИ БАШКОРТОСТАН "ДВОРЕЦ БОРЬБЫ"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ ОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ ДОПОЛНИТЕЛЬНОГО ОБРАЗОВАНИЯ "СПОРТИВНАЯ ШКОЛА ОЛИМПИЙСКОГО РЕЗЕРВА № 4"</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Поставка комплекта воздушных фильтров для приточно-вытяжных установок системы вентиляции и кондиционирования ГАУ ЦСП РБ «Дворец борьбы»</t>
+          <t>Оказание услуг по механизированной уборке снега парковки для транспорта</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>100 665,33 ₽</t>
+          <t>207 000,00 ₽</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
+          <t>07.11.2025, 07.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18997019</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18988092</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>№ 32515344335</t>
+          <t>№ 32515377829</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ "ГОРОДСКАЯ БОЛЬНИЦА № 2 Г. МАГНИТОГОРСК"</t>
+          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ ФИЗИЧЕСКОЙ КУЛЬТУРЫ И СПОРТА ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР СПОРТИВНОЙ ПОДГОТОВКИ"</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Поставка изделий медицинского назначения</t>
+          <t>Поставка наградной атрибутики - кубки</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>585 214,00 ₽</t>
+          <t>111 780,00 ₽</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>28.10.2025, 10.11.2025, 17.11.2025</t>
+          <t>07.11.2025, 07.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18997108</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18987232</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>№ 32515384358</t>
+          <t>№ 32515377316</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "ТОГУЧИНСКОЕ АВТОТРАНСПОРТНОЕ ПРЕДПРИЯТИЕ"</t>
+          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "БЛАГОУСТРОЙСТВО"</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Поставка горюче-смазочных материалов (ГСМ) с использованием пластиковых топливных карт через сеть АЗС</t>
+          <t>Выполнение работ капитального ремонта по замене розлива холодного водоснабжения в многоквартирном доме по адресу: Вологодская область п. Шексна ул. Исполкомовская д. 17</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>15 000 000,00 ₽</t>
+          <t>650 000,00 ₽</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 26.11.2025</t>
+          <t>07.11.2025, 07.11.2025, 07.11.2025</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1716,34 +1724,34 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995922</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18986721</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>№ 32515383805</t>
+          <t>№ 32515374600</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ "ГОРОДСКАЯ БОЛЬНИЦА № 4"</t>
+          <t>МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ "ЧЕРЕПОВЕЦКАЯ АВТОКОЛОННА № 1456"</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Оказание услуги по проведению бактериологических исследований для нужд отделения платных услуг ГБУЗ «Городская больница №4»</t>
+          <t>Поставка горюче-смазочных материалов (ГСМ) на декабрь</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>200 000,00 ₽</t>
+          <t>17 000 000,00 ₽</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 17.11.2025</t>
+          <t>06.11.2025, 06.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1753,293 +1761,293 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995329</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18983271</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>№ 32515385336</t>
+          <t>№ 32515374403</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ СВЕРДЛОВСКОЙ ОБЛАСТИ "СВЕРДЛОВСКИЙ ОБЛАСТНОЙ ЦЕНТР ПРОФИЛАКТИКИ И БОРЬБЫ СО СПИД"</t>
+          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "ВОЛОГОДСКАЯ ОБЛАСТНАЯ ЭНЕРГЕТИЧЕСКАЯ КОМПАНИЯ"</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Многофункциональные устройства и картриджи</t>
+          <t>Право заключения договора на поставку масла отработанного, очищенного в качестве топлива для котельной ЖБИ ТУ «Устюжна» АО «Вологдаоблэнерго».</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1 271 875,00 ₽</t>
+          <t>2 495 416,67 ₽</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
+          <t>06.11.2025, 06.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Запрос предложений в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18997101</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18983002</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>№ 32515385332</t>
+          <t>№ 32515374221</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ ЦЕНТР СПОРТИВНОЙ ПОДГОТОВКИ РЕСПУБЛИКИ БАШКОРТОСТАН "ДВОРЕЦ БОРЬБЫ"</t>
+          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "ВОЛОГОДСКАЯ ОБЛАСТНАЯ ЭНЕРГЕТИЧЕСКАЯ КОМПАНИЯ"</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Оказание услуг по комплексному техническому обслуживанию лифтов и эскалаторов ГАУ ЦСП РБ «Дворец борьбы»</t>
+          <t>Право заключения договора на поставку материалов для монтажа провода для нужд АО «Вологдаоблэнерго».</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>793 920,00 ₽</t>
+          <t>8 000 000,00 ₽</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
+          <t>06.11.2025, 06.11.2025, 18.11.2025</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Прочие</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996962</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18982832</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>№ 32515385330</t>
+          <t>№ 32515354612</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "БАШКИРСКАЯ ГЕНЕРИРУЮЩАЯ КОМПАНИЯ"</t>
+          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "УЧЕБНО-ОПЫТНЫЙ МОЛОЧНЫЙ ЗАВОД" ВОЛОГОДСКОЙ ГОСУДАРСТВЕННОЙ МОЛОЧНОХОЗЯЙСТВЕННОЙ АКАДЕМИИ ИМЕНИ Н.В. ВЕРЕЩАГИНА"</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>220938 Техническое обслуживание ЧРП-6 кВ механизмов собственных нужд для Салаватской ТЭЦ филиала ООО "БГК"</t>
+          <t>Поставка молока коровьего сырого</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2 473 699,40 ₽</t>
+          <t>435 888 000,00 ₽</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
+          <t>30.10.2025, 06.11.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>223-ФЗ Конкурс в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18997082</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18981000</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>№ 32515385324</t>
+          <t>№ 32515372204</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "СЕВЕРРЕЧФЛОТ"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ ОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ ДОПОЛНИТЕЛЬНОГО ОБРАЗОВАНИЯ "СПОРТИВНАЯ ШКОЛА "СПОРТИВНЫЙ КЛУБ ЧЕРЕПОВЕЦ"</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Поставка запчастей для двигателя 6 ЧН21/21</t>
+          <t>Поставка нефтепродуктов</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1 260 027,60 ₽</t>
+          <t>432 000,00 ₽</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 17.11.2025</t>
+          <t>05.11.2025, 05.11.2025</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Прочие</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996848</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18980084</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>№ 32515385323</t>
+          <t>№ 32515371730</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО ТЕЛЕРАДИОВЕЩАТЕЛЬНАЯ КОМПАНИЯ "БАШКОРТОСТАН"</t>
+          <t>ФЕДЕРАЛЬНОЕ БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ "ЦЕНТР ГИГИЕНЫ И ЭПИДЕМИОЛОГИИ В ВОЛОГОДСКОЙ ОБЛАСТИ"</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Оказание услуг по изготовлению декорации для организации трансляции «Прямой линии» с Главой Республики Башкортостан Радием Фаритовичем Хабировым</t>
+          <t>Поставка установки химической деконтаминации стоков</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>787 176,00 ₽</t>
+          <t>184 593,33 ₽</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>05.11.2025, 05.11.2025, 13.11.2025</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18997068</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18979415</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>№ 32515385315</t>
+          <t>№ 32515352239</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ ЦЕНТР СПОРТИВНОЙ ПОДГОТОВКИ РЕСПУБЛИКИ БАШКОРТОСТАН "ДВОРЕЦ БОРЬБЫ"</t>
+          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "УЧЕБНО-ОПЫТНЫЙ МОЛОЧНЫЙ ЗАВОД" ВОЛОГОДСКОЙ ГОСУДАРСТВЕННОЙ МОЛОЧНОХОЗЯЙСТВЕННОЙ АКАДЕМИИ ИМЕНИ Н.В. ВЕРЕЩАГИНА"</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Оказание услуг по охране объектов и имущества ГАУ ЦСП РБ «Дворец борьбы»</t>
+          <t>Поставка молока коровьего сырого</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>15 330 000,00 ₽</t>
+          <t>146 850 000,00 ₽</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
+          <t>29.10.2025, 05.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>223-ФЗ Конкурс в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18997071</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18978498</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>№ 32515382655</t>
+          <t>№ 32515367552</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ПУБЛИЧНОЕ АКЦИОНЕРНОЕ ОБЩЕСТВО ЭНЕРГЕТИКИ И ЭЛЕКТРИФИКАЦИИ "САХАЛИНЭНЕРГО"</t>
+          <t>МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ ВОДОПРОВОДНО-КАНАЛИЗАЦИОННОГО ХОЗЯЙСТВА Г. ВЕЛИКИЙ УСТЮГ</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ОКПД2 28.11.42.000 Поставка оборудования для газотурбинной установки для нужд ОП "Южно-Сахалинская ТЭЦ-1" (Лот № 0136-РЕМ ПРОД-2026-СЭ)</t>
+          <t>Поставка люков чугунных для нужд МУП «Водоканал» г. Великий Устюг</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>23 141 032,07 ₽</t>
+          <t>496 550,60 ₽</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 20.11.2025</t>
+          <t>01.11.2025, 05.11.2025, 10.11.2025</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18993729</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18976084</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>№ 32515382654</t>
+          <t>№ 32515369628</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>МАГАДАНСКОЕ ОБЛАСТНОЕ ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ ПРОФЕССИОНАЛЬНОЕ ОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ "КОЛЛЕДЖ СЕРВИСА И ТЕХНОЛОГИЙ"</t>
+          <t>МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ ГОРОДА ЧЕРЕПОВЦА "ЭЛЕКТРОСЕТЬ"</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Физическая охрана</t>
+          <t>Поставка счетчиков электроэнергии</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>865 920,00 ₽</t>
+          <t>339 600,00 ₽</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>05.11.2025, 05.11.2025, 13.11.2025</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2049,145 +2057,145 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18993732</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18976840</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>№ 32515385306</t>
+          <t>№ 32515339717</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>СУРГУТСКОЕ ГОРОДСКОЕ МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ "ГОРОДСКИЕ ТЕПЛОВЫЕ СЕТИ"</t>
+          <t>МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ ЖИЛИЩНО-КОММУНАЛЬНОГО ХОЗЯЙСТВА ГОРОДСКОГО ОКРУГА ГОРОДА ВОЛОГДЫ "ВОЛОГДАГОРВОДОКАНАЛ"</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Поставка мясной продукции</t>
+          <t>Поставка стола-мойки лабораторной химической</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>3 003 668,00 ₽</t>
+          <t>297 278,00 ₽</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 17.11.2025</t>
+          <t>27.10.2025, 01.11.2025, 10.11.2025</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Прочие</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996878</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18973845</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>№ 32515364218</t>
+          <t>№ 32515367490</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "САХАТРАНСНЕФТЕГАЗ"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ КУЛЬТУРЫ "ДВОРЕЦ ХИМИКОВ"</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Комплекс работ по лесовосстановлению на 22,7947 га для объекта: "Межпоселковый газопровод Бедимя-Сымах Мегино-Кангаласского улуса"</t>
+          <t>Услуги по поставке: Флаг России, без герба; черенок для уборочного инвентаря, деревянный (эвкалипт) лакированный на организацию и проведение городского культурно-массового мероприятия, посвященного Дню народного единства и Дню города: городское мероприятие «Город нашей судьбы и надежды».</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>7 313 299,58 ₽</t>
+          <t>145 500,00 ₽</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>01.11.2025, 10.11.2025, 19.11.2025</t>
+          <t>01.11.2025, 01.11.2025</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Закупка у единственного поставщика (подрядчика, исполнителя)</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994775</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18973732</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>№ 32515385281</t>
+          <t>№ 32515367295</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>МУНИЦИПАЛЬНОЕ ДОШКОЛЬНОЕ ОБРАЗОВАТЕЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ "ДЕТСКИЙ САД № 116"</t>
+          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "ВОЛОГДАГОРТЕПЛОСЕТЬ"</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Оказание услуг по физической охране</t>
+          <t>Выполнение работ по строительству участка тепловой сети ТК-24АЮ-4-1 (вблизи ул. С.Преминина, 4) - ул. Планерная, 14, 16</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1 457 664,00 ₽</t>
+          <t>84 162 585,68 ₽</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 17.11.2025</t>
+          <t>01.11.2025, 01.11.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18997047</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18973504</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>№ 32515305177</t>
+          <t>№ 32515367249</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "КРАСНОЯРСКИЙ РЕЧНОЙ ПОРТ"</t>
+          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "ЭЛИС"</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Поставка бензина АИ-92 и АИ-98 по топливным картам для автотранспорта и хозяйственных нужд АО «КРП»</t>
+          <t>Заключение договора на поставку спецодежды</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1 037 175,00 ₽</t>
+          <t>311 044,00 ₽</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>15.10.2025, 10.11.2025, 14.11.2025</t>
+          <t>01.11.2025, 01.11.2025, 12.11.2025</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2197,30 +2205,34 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995838</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18973401</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>№ 32515383389</t>
+          <t>№ 32515367044</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "САХАЭНЕРГО"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ ОБЩЕОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ "СРЕДНЯЯ ОБЩЕОБРАЗОВАТЕЛЬНАЯ ШКОЛА №33"</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ОКПД2 - 64.19.21.000. Кредитная линия (Лоты № 3001-ФИН ФД-2026-СахаЭ, № 3002-ФИН ФД-2026-СахаЭ)</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr"/>
+          <t>Поставка моноблока для нужд МАОУ "СОШ №33"</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>350 000,00 ₽</t>
+        </is>
+      </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 03.12.2025</t>
+          <t>01.11.2025, 01.11.2025, 12.11.2025</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2230,71 +2242,71 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994765</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18973276</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>№ 32515385267</t>
+          <t>№ 32515367035</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "БАШКИРСКАЯ ГЕНЕРИРУЮЩАЯ КОМПАНИЯ"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ ОБЩЕОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ "СРЕДНЯЯ ОБЩЕОБРАЗОВАТЕЛЬНАЯ ШКОЛА №33"</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>220933_Поставка обеспечения программного Антивирус для виртуальных сред для ООО "БГК"</t>
+          <t>Поставка интера??ктивного программно-аппаратного комплекса с рельсовой системой</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1 453 636,00 ₽</t>
+          <t>2 040 000,00 ₽</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
+          <t>01.11.2025, 01.11.2025, 11.11.2025</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18997015</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18973183</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>№ 32515385264</t>
+          <t>№ 32515366963</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ ОБЩЕОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ "БЕЛОЯРСКАЯ СРЕДНЯЯ ОБЩЕОБРАЗОВАТЕЛЬНАЯ ШКОЛА № 1"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ ОБЩЕОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ "СРЕДНЯЯ ОБЩЕОБРАЗОВАТЕЛЬНАЯ ШКОЛА №33"</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Выполнение работ по ремонту уличного освещения</t>
+          <t>Поставка оборудования для кабинета физики для нужд МАОУ "СОШ №33"</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>388 699,96 ₽</t>
+          <t>505 000,00 ₽</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>01.11.2025, 01.11.2025, 12.11.2025</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2304,145 +2316,145 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18997013</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18973120</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>№ 32515385104</t>
+          <t>№ 32515366899</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО ТЕЛЕРАДИОВЕЩАТЕЛЬНАЯ КОМПАНИЯ "БАШКОРТОСТАН"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ ОБЩЕОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ "СРЕДНЯЯ ОБЩЕОБРАЗОВАТЕЛЬНАЯ ШКОЛА №33"</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Оказание услуг по техническому обслуживанию трансляции «Прямой линии» с Главой Республики Башкортостан Радием Фаритовичем Хабировым</t>
+          <t>Поставка оборудования для кабинета географии для нужд МАОУ "СОШ?? №33"</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>275 000,00 ₽</t>
+          <t>40 200,00 ₽</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>01.11.2025, 01.11.2025, 11.11.2025</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18997023</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18973092</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>№ 32515377491</t>
+          <t>№ 32515355422</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ "РЕСПУБЛИКАНСКАЯ КЛИНИЧЕСКАЯ БОЛЬНИЦА ИМ. Н.А.СЕМАШКО" МИНИСТЕРСТВА ЗДРАВООХРАНЕНИЯ РЕСПУБЛИКИ БУРЯТИЯ</t>
+          <t>МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ "КОММУНАЛЬНЫЕ СИСТЕМЫ"</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Поставка сетчатых имплантов для хирургического отделения на 2026 год (для субъектов малого и среднего предпринимательства)</t>
+          <t>выполнение работ по техническому перевооружению опасного производственного объекта "склад хлора" (включая хлораторное отделение) рег. №А28-02272-0001 в части установки на трубопроводе газообразного хлора запорной арматуры с электроприводом с дистанционным управлением для нужд МУП "Коммунальные системы"</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>3 338 880,00 ₽</t>
+          <t>692 494,88 ₽</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>07.11.2025, 10.11.2025, 18.11.2025</t>
+          <t>30.10.2025, 01.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Прочие</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995122</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18972324</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>№ 32515385250</t>
+          <t>№ 32515365867</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ СВЕРДЛОВСКОЙ ОБЛАСТИ "ТУГУЛЫМСКАЯ ЦЕНТРАЛЬНАЯ РАЙОННАЯ БОЛЬНИЦА"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ КУЛЬТУРЫ "ДВОРЕЦ МЕТАЛЛУРГОВ"</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Приобретение хлеба свежего (недлительного хранения) для нужд ГАУЗ СО "Тугулымская ЦРБ" на период с декабря 2025 года до мая 2026 года.</t>
+          <t>Поставка Ноутбук Apple MacBook Air</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>438 606,00 ₽</t>
+          <t>66 280,00 ₽</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 17.11.2025</t>
+          <t>01.11.2025, 01.11.2025, 11.11.2025</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Прочие</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18997004</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18971546</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>№ 32515345739</t>
+          <t>№ 32515365741</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "АЭРОПОРТ ЕМЕЛЬЯНОВО"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ КУЛЬТУРЫ "ДВОРЕЦ МЕТАЛЛУРГОВ"</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Выполнение работ по разработке рабочей документации по оборудованию специальными техническими средствами обнаружения и противодействия беспилотным летательным аппаратам в Международном аэропорту Красноярск</t>
+          <t>Поставка Ламп а театральные прожектора</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>12 000 000,00 ₽</t>
+          <t>230 055,96 ₽</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>28.10.2025, 10.11.2025, 14.11.2025</t>
+          <t>01.11.2025, 01.11.2025, 11.11.2025</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -2452,219 +2464,219 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995760</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18971369</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>№ 32515383358</t>
+          <t>№ 32515362529</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ АМУРСКОЙ ОБЛАСТИ "МАЗАНОВСКИЙ ДОМ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ"</t>
+          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "ВОЛОГДАГОРТЕПЛОСЕТЬ"</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Поставка полотенец махровых</t>
+          <t>Поставка блочного вакуумного деаэратора БВД-15</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>125 441,40 ₽</t>
+          <t>5 499 933,33 ₽</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 17.11.2025</t>
+          <t>31.10.2025, 31.10.2025, 10.11.2025</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994462</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18967802</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>№ 32515383357</t>
+          <t>№ 32515362450</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ АМУРСКОЙ ОБЛАСТИ "БЕЛОГОРСКИЙ ДОМ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ"</t>
+          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "ВОЛОГДАГОРТЕПЛОСЕТЬ"</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Поставка муки ржаной</t>
+          <t>Поставка бумаги для офисной техники</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>97 500,00 ₽</t>
+          <t>843 333,33 ₽</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
+          <t>31.10.2025, 31.10.2025, 10.11.2025</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994674</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18967703</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>№ 32515383705</t>
+          <t>№ 32515362117</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>ОБЛАСТНОЕ ГОСУДАРСТВЕННОЕ БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ "ПУЛЯЕВСКИЙ ДОМ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ"</t>
+          <t>ФЕДЕРАЛЬНОЕ БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ "ЦЕНТР ГИГИЕНЫ И ЭПИДЕМИОЛОГИИ В ВОЛОГОДСКОЙ ОБЛАСТИ"</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Поставка фруктов</t>
+          <t>Транспортно-экспедиционные услуги, в том числе связанные с приемом, обработкой, хранением, упаковкой, перевозкой, доставкой грузов по территории РФ и других государств, организацией страхования и таможенного оформления грузов</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>4 548 345,00 ₽</t>
+          <t>300 000,00 ₽</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
+          <t>31.10.2025, 31.10.2025, 31.10.2025</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Прочие</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995169</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18967285</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>№ 32515379622</t>
+          <t>№ 32515362057</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>ФЕДЕРАЛЬНОЕ ГОСУДАРСТВЕННОЕ БЮДЖЕТНОЕ ОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ ВЫСШЕГО ОБРАЗОВАНИЯ "ЗАПОЛЯРНЫЙ ГОСУДАРСТВЕННЫЙ УНИВЕРСИТЕТ ИМ. Н.М. ФЕДОРОВСКОГО"</t>
+          <t>МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ ЖИЛИЩНО-КОММУНАЛЬНОГО ХОЗЯЙСТВА ГОРОДСКОГО ОКРУГА ГОРОДА ВОЛОГДЫ "ВОЛОГДАГОРВОДОКАНАЛ"</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Поставка планшетных компьютеров</t>
+          <t>Поставка горюче-смазочных материалов с АЗС по топливным картам</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>656 746,67 ₽</t>
+          <t>45 648 500,00 ₽</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>07.11.2025, 10.11.2025, 14.11.2025</t>
+          <t>31.10.2025, 31.10.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Прочие</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995752</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18967204</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>№ 32515383351</t>
+          <t>№ 32515361960</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ АМУРСКОЙ ОБЛАСТИ "БЕЛОГОРСКИЙ ДОМ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ"</t>
+          <t>ФЕДЕРАЛЬНОЕ БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ "ЦЕНТР ГИГИЕНЫ И ЭПИДЕМИОЛОГИИ В ВОЛОГОДСКОЙ ОБЛАСТИ"</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Поставка муки высшего сорта</t>
+          <t>Техническое обслуживание и ремонт систем вентиляции и кондиционирования воздуха</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>630 000,00 ₽</t>
+          <t>132 000,00 ₽</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
+          <t>31.10.2025, 31.10.2025, 31.10.2025</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Прочие</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994667</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18967072</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>№ 32515385214</t>
+          <t>№ 32515361887</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО САНАТОРИЙ "АССЫ"</t>
+          <t>ФЕДЕРАЛЬНОЕ БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ "ЦЕНТР ГИГИЕНЫ И ЭПИДЕМИОЛОГИИ В ВОЛОГОДСКОЙ ОБЛАСТИ"</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Поставка новогодних кондитерских изделий (подарочные наборы)</t>
+          <t>Поставка сувенирной продукции (календари, пакеты)</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>355 932,70 ₽</t>
+          <t>109 800,00 ₽</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
+          <t>31.10.2025, 31.10.2025, 31.10.2025</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -2674,34 +2686,34 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996972</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18966957</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>№ 32515384203</t>
+          <t>№ 32515361817</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>ОБЛАСТНОЕ ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ КУЛЬТУРЫ "ТОМСКАЯ ОБЛАСТНАЯ ГОСУДАРСТВЕННАЯ ФИЛАРМОНИЯ"</t>
+          <t>МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ ЖИЛИЩНО-КОММУНАЛЬНОГО ХОЗЯЙСТВА ГОРОДСКОГО ОКРУГА ГОРОДА ВОЛОГДЫ "ВОЛОГДАГОРВОДОКАНАЛ"</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Поставка искусственной ели</t>
+          <t>Выполнение работ по восстановлению нарушенного благоустройства после проведения аварийных работ на сетях МУП ЖКХ «Вологдагорводоканал»</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>139 650,00 ₽</t>
+          <t>2 999 919,04 ₽</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>31.10.2025, 31.10.2025</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -2711,34 +2723,34 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995771</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18966893</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>№ 32515384681</t>
+          <t>№ 32515360646</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ОМСКОЙ ОБЛАСТИ ДОПОЛНИТЕЛЬНОГО ОБРАЗОВАНИЯ "СПОРТИВНАЯ ШКОЛА ОЛИМПИЙСКОГО РЕЗЕРВА ПО ХУДОЖЕСТВЕННОЙ ГИМНАСТИКЕ"</t>
+          <t>ФЕДЕРАЛЬНОЕ ГОСУДАРСТВЕННОЕ БЮДЖЕТНОЕ ОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ ВЫСШЕГО ОБРАЗОВАНИЯ "ВОЛОГОДСКИЙ ГОСУДАРСТВЕННЫЙ УНИВЕРСИТЕТ"</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Поставка электрических чайников</t>
+          <t>Спорттовары</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>4 197,00 ₽</t>
+          <t>240 815,00 ₽</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 11.11.2025</t>
+          <t>31.10.2025, 31.10.2025</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -2748,182 +2760,182 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996309</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18964981</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>№ 32515385203</t>
+          <t>№ 32515359713</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ ХАНТЫ-МАНСИЙСКОГО АВТОНОМНОГО ОКРУГА - ЮГРЫ "ЮГРАМЕГАСПОРТ"</t>
+          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "ЦЕНТР 112"</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Оказание услуг по организации проживания в гостинице на территории г. Югорска участников Международных соревнований по боксу "Кубок нефтяных стран, посвященный памяти Героя Социалистического Труда Ф.К. Салманова" (ЗКЭ-393.25)</t>
+          <t>Дерматологические средства индивидуальной защиты</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>191 800,00 ₽</t>
+          <t>888 400,00 ₽</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 17.11.2025</t>
+          <t>31.10.2025, 31.10.2025, 31.10.2025</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Прочие</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996949</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18963969</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>№ 32515343051</t>
+          <t>№ 32515359260</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ КУЛЬТУРЫ СВЕРДЛОВСКОЙ ОБЛАСТИ "СВЕРДЛОВСКИЙ ГОСУДАРСТВЕННЫЙ АКАДЕМИЧЕСКИЙ ТЕАТР МУЗЫКАЛЬНОЙ КОМЕДИИ"</t>
+          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ ФИЗИЧЕСКОЙ КУЛЬТУРЫ И СПОРТА ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР СПОРТИВНОЙ ПОДГОТОВКИ"</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Оказание полиграфических услуг и изготовление печатной продукции</t>
+          <t>Поставка рамок</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>7 771 957,00 ₽</t>
+          <t>71 400,00 ₽</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>27.10.2025, 10.11.2025, 07.11.2025</t>
+          <t>31.10.2025, 31.10.2025, 11.11.2025</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996874</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18963629</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>№ 32515385197</t>
+          <t>№ 32515311134</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ "ДВОРЕЦ СПОРТА "ЗВЕЗДНЫЙ"</t>
+          <t>МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ "ЧЕРЕПОВЕЦКАЯ АВТОКОЛОННА № 1456"</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Изготовление и поставка рулонных штор для нужд МАУ «ДС «Звездный»</t>
+          <t>поставка ГСМ с использованием пластиковых карт через сеть АЗС</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>453 000,00 ₽</t>
+          <t>30 000 000,00 ₽</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 17.11.2025</t>
+          <t>17.10.2025, 31.10.2025, 07.11.2025</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Прочие</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18997307</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18963557</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>№ 32515385195</t>
+          <t>№ 32515357648</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ СТАЦИОНАРНОЕ УЧРЕЖДЕНИЕ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ "ПОЛЕТАЕВСКИЙ ПСИХОНЕВРОЛОГИЧЕСКИЙ ИНТЕРНАТ"</t>
+          <t>МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ ЖИЛИЩНО-КОММУНАЛЬНОГО ХОЗЯЙСТВА ГОРОДСКОГО ОКРУГА ГОРОДА ВОЛОГДЫ "ВОЛОГДАГОРВОДОКАНАЛ"</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Поставка продуктов питания ( чай ,кисель, какао-порошок, кофейный напиток)</t>
+          <t>Оказание услуг почтовой связи</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>38 861,63 ₽</t>
+          <t>1 000 000,00 ₽</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 14.11.2025</t>
+          <t>30.10.2025, 30.10.2025, 10.11.2025</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Прочие</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996951</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18961484</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>№ 32515385190</t>
+          <t>№ 32515357583</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО ТЕЛЕРАДИОВЕЩАТЕЛЬНАЯ КОМПАНИЯ "БАШКОРТОСТАН"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ КУЛЬТУРЫ "ДИРЕКЦИЯ КОНЦЕРТНО-ЗРЕЛИЩНЫХ ПРЕДСТАВЛЕНИЙ И ПРАЗДНИКОВ ГОРОДА ВОЛОГДЫ"</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Оказание услуг по техническому обслуживанию трансляции «Прямой линии» с Главой Республики Башкортостан Радием Фаритовичем Хабировым с применением собственного оборудования</t>
+          <t>Услуги по организации выступления кавер-группы «Патифоникс» (г. Ярославль) на концерте в рамках новогодних и рождественских праздничных мероприятий 2025-2026 годов</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>670 497,08 ₽</t>
+          <t>319 000,00 ₽</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>30.10.2025, 30.10.2025</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -2933,108 +2945,108 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996940</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18961499</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>№ 32515385179</t>
+          <t>№ 32515357564</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ "ДВОРЕЦ КУЛЬТУРЫ МЕТАЛЛУРГОВ"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ КУЛЬТУРЫ "ДИРЕКЦИЯ КОНЦЕРТНО-ЗРЕЛИЩНЫХ ПРЕДСТАВЛЕНИЙ И ПРАЗДНИКОВ ГОРОДА ВОЛОГДЫ"</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>оказание услуг частной охраны (выставление поста охраны)</t>
+          <t>Услуги по организации двух спектаклей «Декаданс» на фестивале уличных театров в рамках новогодних и рождественских праздничных мероприятий 2025-2026 годов с участием театра «Странствующие Куклы Господина Пэжо»</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2 102 400,00 ₽</t>
+          <t>530 000,00 ₽</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
+          <t>30.10.2025, 30.10.2025</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Прочие</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996938</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18961475</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>№ 32515353169</t>
+          <t>№ 32515357408</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "УСТЬ-СРЕДНЕКАНГЭССТРОЙ"</t>
+          <t>МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ ВОДОПРОВОДНО-КАНАЛИЗАЦИОННОГО ХОЗЯЙСТВА Г. ВЕЛИКИЙ УСТЮГ</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>ОКПД2 27.12.31.000 Поставка, шефмонтаж, шефналадка распределительного устройства собственных нужд 0,4 кВ и силовых сухих трансформаторов 6/0,4 кВ для объекта капитального строительства – здание химводоочистки в рамках выполнения генподрядных работ для реализации проекта «Строительство Хабаровской ТЭЦ-4 с внеплощадочной инфраструктурой.» 2.1 Этап (Лот № 0696-КС ДОХ-2025-УСГС)</t>
+          <t>Поставка средств индивидуальной защиты (спецобувь) для нужд МУП "Водоканал" г. Великий Устюг</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>34 790 000,00 ₽</t>
+          <t>366 400,74 ₽</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>30.10.2025, 10.11.2025, 17.11.2025</t>
+          <t>30.10.2025, 30.10.2025, 07.11.2025</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994026</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18961294</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>№ 32515384164</t>
+          <t>№ 32515357288</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>ФЕДЕРАЛЬНОЕ ГОСУДАРСТВЕННОЕ БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ "НАЦИОНАЛЬНЫЙ МЕДИЦИНСКИЙ ИССЛЕДОВАТЕЛЬСКИЙ ЦЕНТР ИМЕНИ АКАДЕМИКА Е.Н. МЕШАЛКИНА" МИНИСТЕРСТВА ЗДРАВООХРАНЕНИЯ РОССИЙСКОЙ ФЕДЕРАЦИИ</t>
+          <t>ФЕДЕРАЛЬНОЕ ГОСУДАРСТВЕННОЕ БЮДЖЕТНОЕ ОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ ВЫСШЕГО ОБРАЗОВАНИЯ "ВОЛОГОДСКИЙ ГОСУДАРСТВЕННЫЙ УНИВЕРСИТЕТ"</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Поставка лабораторных животных (свиньи)</t>
+          <t>Работы по текущему ремонту 333 аудитории корпуса № 1</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>104 670,00 ₽</t>
+          <t>1 500 000,00 ₽</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>30.10.2025, 30.10.2025</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -3044,219 +3056,219 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994247</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18961106</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>№ 32515383671</t>
+          <t>№ 32515357182</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>ОБЛАСТНОЕ ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ "ИРКУТСКАЯ ГОРОДСКАЯ КЛИНИЧЕСКАЯ БОЛЬНИЦА № 8"</t>
+          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "ШЕКСНА-ТЕПЛОСЕТЬ"</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Поставка полотенец бумажных листовых для диспенсера</t>
+          <t>Поставка термоусаживаемых муфт для стыковки труб ППУ ПЭ 159/250</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>615 600,00 ₽</t>
+          <t>8 960,00 ₽</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 17.11.2025</t>
+          <t>30.10.2025, 30.10.2025</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Закупка у единственного поставщика (подрядчика, исполнителя)</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995114</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18960984</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>№ 32515385159</t>
+          <t>№ 32515357071</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>МУНИЦИПАЛЬНОЕ ОБЩЕОБРАЗОВАТЕЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ "СРЕДНЯЯ ОБЩЕОБРАЗОВАТЕЛЬНАЯ ШКОЛА № 18"</t>
+          <t>МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ ГОРОДА ЧЕРЕПОВЦА " ЭЛЕКТРОТРАНС"</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Оказание услуг по физической охране</t>
+          <t>Поставка кузовных деталей трамвайного вагона.</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>1 457 664,00 ₽</t>
+          <t>143 281,00 ₽</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 17.11.2025</t>
+          <t>30.10.2025, 30.10.2025</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Закупка у единственного поставщика (подрядчика, исполнителя)</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996922</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18960843</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>№ 32515358402</t>
+          <t>№ 32515356948</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>ПУБЛИЧНОЕ АКЦИОНЕРНОЕ ОБЩЕСТВО ЭНЕРГЕТИКИ И ЭЛЕКТРИФИКАЦИИ "МАГАДАНЭНЕРГО"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ ОБЩЕОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ СЯМЖЕНСКОГО МУНИЦИПАЛЬНОГО ОКРУГА "СЯМЖЕНСКАЯ СРЕДНЯЯ ШКОЛА"</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>ОКПД2 26.40.33 Приобретение комплектующих для ремонта систем видеонаблюдения для нужд филиалов ПАО "Магаданэнерго"</t>
+          <t>поставка товара</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>1 008 288,15 ₽</t>
+          <t>286 780,00 ₽</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>31.10.2025, 10.11.2025, 14.11.2025</t>
+          <t>30.10.2025, 30.10.2025</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Закупка у единственного поставщика (подрядчика, исполнителя)</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18993547</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18960680</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>№ 32515385154</t>
+          <t>№ 32515356895</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "НОВАЯ ГОРОДСКАЯ ИНФРАСТРУКТУРА ПРИКАМЬЯ"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ ОБЩЕОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ СЯМЖЕНСКОГО МУНИЦИПАЛЬНОГО ОКРУГА "СЯМЖЕНСКАЯ СРЕДНЯЯ ШКОЛА"</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Ремонт внутренних помещений сметного и технического отдела в здании гаража производственной базы по адресу: г. Пермь, ул. Фрезеровщиков 50</t>
+          <t>поставка товара</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>4 755 865,35 ₽</t>
+          <t>307 945,00 ₽</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 19.11.2025</t>
+          <t>30.10.2025, 30.10.2025</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>223-ФЗ Конкурс в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Прочие</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996908</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18840863</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>№ 32515385153</t>
+          <t>№ 32515356328</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ СВЕРДЛОВСКОЙ ОБЛАСТИ "ТУГУЛЫМСКАЯ ЦЕНТРАЛЬНАЯ РАЙОННАЯ БОЛЬНИЦА"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ ОБЩЕОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ "СРЕДНЯЯ ОБЩЕОБРАЗОВАТЕЛЬНАЯ ШКОЛА № 36"</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Приобретение продуктов питания (иные, бакалея) для нужд ГАУЗ СО "Тугулымская ЦРБ" на период с декабря 2025 года по февраль 2026 года.</t>
+          <t>Работы по разработке дизайн-проекта интерьеров помещений</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>231 715,34 ₽</t>
+          <t>300 000,00 ₽</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 17.11.2025</t>
+          <t>30.10.2025, 30.10.2025</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Закупка у единственного поставщика (подрядчика, исполнителя)</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996710</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18959809</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>№ 32515385152</t>
+          <t>№ 32515355156</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ ДОПОЛНИТЕЛЬНОГО ОБРАЗОВАНИЯ ГОРОДА НЯГАНИ "СПОРТИВНАЯ ШКОЛА ОЛИМПИЙСКОГО РЕЗЕРВА "ЦЕНТР СПОРТИВНОЙ ПОДГОТОВКИ"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ "ЦЕНТР МУНИЦИПАЛЬНЫХ ИНФОРМАЦИОННЫХ РЕСУРСОВ И ТЕХНОЛОГИЙ"</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Поставка каленного стекла</t>
+          <t>Поставка маршрутизатора</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>291 394,00 ₽</t>
+          <t>9 600,00 ₽</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
+          <t>30.10.2025, 30.10.2025</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -3266,145 +3278,145 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996850</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18958268</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>№ 32515342958</t>
+          <t>№ 32515355145</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ ДОПОЛНИТЕЛЬНОГО ОБРАЗОВАНИЯ СПОРТИВНАЯ ШКОЛА ОЛИМПИЙСКОГО РЕЗЕРВА "ОЛИМП"</t>
+          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ЧЕРЕПОВЕЦКИЙ ДОМ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ"</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Оказание услуг по охране объектов</t>
+          <t>Замена автоматической пожарной сигнализации и системы оповещения и управления эвакуацией в здании спального корпуса по адресу: Вологодская обл., г. Череповец, ул. Ветеранов, д. 12А</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>10 840 500,00 ₽</t>
+          <t>4 928 440,00 ₽</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>27.10.2025, 10.11.2025, 24.11.2025</t>
+          <t>30.10.2025, 30.10.2025, 07.11.2025</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Конкурс в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996899</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18958526</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>№ 32515385151</t>
+          <t>№ 32515354860</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ КУЛЬТУРЫ "ОРЕНБУРГСКАЯ ОБЛАСТНАЯ ФИЛАРМОНИЯ"</t>
+          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ЧЕРЕПОВЕЦКИЙ ДОМ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ"</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>услуги по участию Джаз-квартета «Москва» Олега Киреева в XXVII Международном джаз-фестивале имени Ю. Саульского «Евразия-2025»</t>
+          <t>Замена автоматической пожарной сигнализации и системы оповещения и управления эвакуацией в здании спального корпуса по адресу: Вологодская обл., г. Череповец, ул. Красная, 8</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>189 210,00 ₽</t>
+          <t>5 758 380,00 ₽</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>30.10.2025, 30.10.2025, 07.11.2025</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Конкурс в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996898</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18957959</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>№ 32515339059</t>
+          <t>№ 32515354650</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>ПУБЛИЧНОЕ АКЦИОНЕРНОЕ ОБЩЕСТВО ЭНЕРГЕТИКИ И ЭЛЕКТРИФИКАЦИИ "МАГАДАНЭНЕРГО"</t>
+          <t>МУНИЦИПАЛЬНОЕ БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ "РИТУАЛ-СПЕЦСЛУЖБА"</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>ОКПД2 22.29.21 Поставка электроизоляционных материалов для нужд филиалов ПАО "Магаданэнерго"</t>
+          <t>Поставка кондиционера</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>478 180,73 ₽</t>
+          <t>79 000,00 ₽</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>27.10.2025, 10.11.2025, 14.11.2025</t>
+          <t>30.10.2025, 30.10.2025</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Закупка у единственного поставщика (подрядчика, исполнителя)</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18993553</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18957779</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>№ 32515385149</t>
+          <t>№ 32515354559</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>ФЕДЕРАЛЬНОЕ ГОСУДАРСТВЕННОЕ БЮДЖЕТНОЕ ОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ ВЫСШЕГО ОБРАЗОВАНИЯ "УРАЛЬСКИЙ ГОСУДАРСТВЕННЫЙ ЭКОНОМИЧЕСКИЙ УНИВЕРСИТЕТ"</t>
+          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ КУЛЬТУРЫ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКИЙ ОРДЕНА "ЗНАК ПОЧЕТА" ГОСУДАРСТВЕННЫЙ ДРАМАТИЧЕСКИЙ ТЕАТР"</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Поставка литературы на бумажных и электронных носителях для обучающихся на подготовительном факультете иностранных граждан</t>
+          <t>Выполнение работ по разработке проектной документации на «Капитальный ремонт системы водоснабжения и отопления» в здании театра, расположенном по адресу: г. Вологда, Советский проспект, д.1</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>1 960 000,00 ₽</t>
+          <t>330 000,00 ₽</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>30.10.2025, 30.10.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -3414,34 +3426,34 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996852</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18957663</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>№ 32515384129</t>
+          <t>№ 32515354124</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ РЕСПУБЛИКИ АЛТАЙ "ДИРЕКЦИЯ ЦЕНТРА ИСКУССТВ"</t>
+          <t>МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ ГОРОДА ЧЕРЕПОВЦА "ВОДОКАНАЛ"</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Услуги по поставке систем безопасности, по монтажу и пуско-наладке</t>
+          <t>Концентрат минеральный "Галит" тип С сорт 1</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>1 890 132,00 ₽</t>
+          <t>105 000,00 ₽</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>30.10.2025, 30.10.2025, 06.11.2025</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -3451,71 +3463,71 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995686</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18957173</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>№ 32515384118</t>
+          <t>№ 32515353998</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>ФЕДЕРАЛЬНОЕ ГОСУДАРСТВЕННОЕ БЮДЖЕТНОЕ ОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ ВЫСШЕГО ОБРАЗОВАНИЯ "КРАСНОЯРСКИЙ ГОСУДАРСТВЕННЫЙ ПЕДАГОГИЧЕСКИЙ УНИВЕРСИТЕТ ИМ. В.П. АСТАФЬЕВА"</t>
+          <t>МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ ЖИЛИЩНО-КОММУНАЛЬНОГО ХОЗЯЙСТВА ГОРОДСКОГО ОКРУГА ГОРОДА ВОЛОГДЫ "ВОЛОГДАГОРВОДОКАНАЛ"</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Поставка аккумуляторов</t>
+          <t>Капитальный ремонт вытяжной вентиляции в здании воздуходувок ОСК МУП ЖКХ «Вологдагорводоканал»</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>116 525,00 ₽</t>
+          <t>964 508,40 ₽</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 14.11.2025</t>
+          <t>30.10.2025, 30.10.2025, 07.11.2025</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995593</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18956979</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>№ 32515385141</t>
+          <t>№ 32515353887</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ КУЛЬТУРЫ "ОРЕНБУРГСКАЯ ОБЛАСТНАЯ ФИЛАРМОНИЯ"</t>
+          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ КУЛЬТУРЫ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКИЙ ОРДЕНА "ЗНАК ПОЧЕТА" ГОСУДАРСТВЕННЫЙ ДРАМАТИЧЕСКИЙ ТЕАТР"</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>услуги по участию Евгения Лебедева в XXVII Международном джаз-фестивале имени Ю. Саульского «Евразия-2025»</t>
+          <t>Оказание услуг по охране АУК ВО "Вологодский драматический театр"</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>202 350,00 ₽</t>
+          <t>3 032 250,00 ₽</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>30.10.2025, 30.10.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -3525,34 +3537,34 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996882</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18956797</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>№ 32515360774</t>
+          <t>№ 32515352309</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>КРАЕВОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ ДОПОЛНИТЕЛЬНОГО ПРОФЕССИОНАЛЬНОГО ОБРАЗОВАНИЯ "АЛТАЙСКИЙ ИНСТИТУТ ЦИФРОВЫХ ТЕХНОЛОГИЙ И ОЦЕНКИ КАЧЕСТВА ОБРАЗОВАНИЯ ИМЕНИ ОЛЕГА РОСТИСЛАВОВИЧА ЛЬВОВА"</t>
+          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ ФИЗИЧЕСКОЙ КУЛЬТУРЫ И СПОРТА ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР СПОРТИВНОЙ ПОДГОТОВКИ"</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Оказание услуг по передаче неисключительных (пользовательских) прав на программное обеспечение для серверного оборудования</t>
+          <t>Оказание услуг по специальной оценке условий труда</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>5 516 162,00 ₽</t>
+          <t>50 000,00 ₽</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>31.10.2025, 10.11.2025, 13.11.2025</t>
+          <t>29.10.2025, 29.10.2025, 06.11.2025</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -3562,34 +3574,34 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995679</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18954852</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>№ 32515385129</t>
+          <t>№ 32515351746</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ КУЛЬТУРЫ "ОРЕНБУРГСКАЯ ОБЛАСТНАЯ ФИЛАРМОНИЯ"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ КУЛЬТУРЫ "ДВОРЕЦ МЕТАЛЛУРГОВ"</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Услуги по техническому обслуживанию системы вентиляции</t>
+          <t>Поставка бумаги офисной</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>242 000,00 ₽</t>
+          <t>70 934,00 ₽</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>29.10.2025, 29.10.2025, 06.11.2025</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -3599,71 +3611,71 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996862</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18954111</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>№ 32515355244</t>
+          <t>№ 32515351624</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "ЭН+ ТОРГОВЫЙ ДОМ"</t>
+          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ ДОПОЛНИТЕЛЬНОГО ОБРАЗОВАНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "СПОРТИВНАЯ ШКОЛА ОЛИМПИЙСКОГО РЕЗЕРВА "ВИТЯЗЬ"</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Поставка устройств приема - передачи аварийных сигналов и команд для АО "ИЭСК" ЮЭС</t>
+          <t>Оказание услуг по комплексному обслуживанию инженерных систем теплоснабжения г. В. Устюг в 2026 г.</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>0,00 ₽</t>
+          <t>408 000,00 ₽</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>30.10.2025, 10.11.2025, 20.11.2025</t>
+          <t>29.10.2025, 29.10.2025, 06.11.2025</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995021</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18954020</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>№ 32515385117</t>
+          <t>№ 32515351619</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>СУРГУТСКОЕ ГОРОДСКОЕ МУНИЦИПАЛЬНОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ "ГОРОДСКИЕ ТЕПЛОВЫЕ СЕТИ"</t>
+          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ ДОПОЛНИТЕЛЬНОГО ОБРАЗОВАНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "СПОРТИВНАЯ ШКОЛА ОЛИМПИЙСКОГО РЕЗЕРВА "ВИТЯЗЬ"</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Оказание услуг по адаптации и сопровождению экземпляров систем КонсультантПлюс на основе специального лицензионного сервисного программного обеспечения, обеспечивающего совместимость (взаимодействие) услуг с ранее установленными у заказчика экземплярами систем КонсультантПлюс</t>
+          <t>Оказание услуг по комплексному обслуживанию инженерных систем водоподготовки г.В. Устюг в 2026г.</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>4 119 736,08 ₽</t>
+          <t>408 000,00 ₽</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 17.11.2025</t>
+          <t>29.10.2025, 29.10.2025, 06.11.2025</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -3673,219 +3685,219 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996787</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18953656</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>№ 32515385106</t>
+          <t>№ 32515351464</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ ХАНТЫ-МАНСИЙСКОГО АВТОНОМНОГО ОКРУГА - ЮГРЫ "ОКРУЖНАЯ ТЕЛЕРАДИОКОМПАНИЯ "ЮГРА"</t>
+          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ДОМ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ "СОСНОВАЯ РОЩА"</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Поставка офисной мебели</t>
+          <t>Оказание услуг по охране объекта и имущества, обеспечение внутриобъектового и пропускного режимов в АУ СО ВО «Дом социального обслуживания «Сосновая Роща» с использованием системы видеонаблюдения в период с 01.01.2026 по 30.06.2026 года</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>1 418 244,00 ₽</t>
+          <t>1 918 614,48 ₽</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 17.11.2025</t>
+          <t>29.10.2025, 29.10.2025, 06.11.2025</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Конкурс в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996790</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18953732</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>№ 32515385103</t>
+          <t>№ 32515351447</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ ДОПОЛНИТЕЛЬНОГО ОБРАЗОВАНИЯ НОВОЛЯЛИНСКОГО МУНИЦИПАЛЬНОГО ОКРУГА "ДЕТСКАЯ ШКОЛА ИСКУССТВ ИМЕНИ ОЛЬГИ СТЕПАНОВНЫ БОБКОВОЙ"</t>
+          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "ВОЛОГОДСКАЯ ОБЛАСТНАЯ ЭНЕРГЕТИЧЕСКАЯ КОМПАНИЯ"</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Ремонт входной дверной группы в филиале МАУ ДО НМО "ДШИ им. О.С. Бобковой"</t>
+          <t>Право заключения договора на поставку патронов предохранителей для нужд АО «Вологдаоблэнерго».</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>350 000,00 ₽</t>
+          <t>371 575,47 ₽</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 13.11.2025</t>
+          <t>29.10.2025, 29.10.2025, 07.11.2025</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Запрос предложений в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996840</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18953788</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>№ 32515385100</t>
+          <t>№ 32515351394</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "ВОДОКАНАЛ"</t>
+          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "УЧЕБНО-ОПЫТНЫЙ МОЛОЧНЫЙ ЗАВОД" ВОЛОГОДСКОЙ ГОСУДАРСТВЕННОЙ МОЛОЧНОХОЗЯЙСТВЕННОЙ АКАДЕМИИ ИМЕНИ Н.В. ВЕРЕЩАГИНА"</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Реконструкция самотечной канализации по ул. Метеорологическая от дома № 11 методом горизонтального наклонного бурения протяженностью 330 м с увеличением диметра труб с 200 мм до 250 мм городского поселения г. Мелеуз Республики Башкортостан"</t>
+          <t>Поставка деревянных поддонов</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>4 387 254,00 ₽</t>
+          <t>6 480 000,00 ₽</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
+          <t>29.10.2025, 29.10.2025, 07.11.2025</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996846</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18953718</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>№ 32515385099</t>
+          <t>№ 32515351336</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ ДОШКОЛЬНОЕ ОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ ГОРОДА НЯГАНИ "ДЕТСКИЙ САД №2 "СКАЗКА"</t>
+          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "КОРПОРАЦИЯ РАЗВИТИЯ ВОЛОГОДСКОЙ ОБЛАСТИ"</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>поставка канцелярских товаров</t>
+          <t>Выполнение работ по подготовке территории особой экономической зоны промышленно-производственного типа «Вологодская» на территории Вологодской области к строительству объектов капитального строительства, включающих в себя вырубку зеленых насаждений, очистку мест вырубки от порубочных остатков, складирование древесины, организацию рельефа (вертикальную планировку) земельных участков в границах земельных участков с кадастровыми номерами 35:25:0603074:784, 35:25:0603074:1748, 35:25:0603074:1749.</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>395 928,92 ₽</t>
+          <t>48 950 000,00 ₽</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 17.11.2025</t>
+          <t>29.10.2025, 29.10.2025</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Закупка у единственного поставщика (подрядчика, исполнителя)</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996764</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18953540</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>№ 32515385096</t>
+          <t>№ 32515351106</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ХАНТЫ-МАНСИЙСКОГО АВТОНОМНОГО ОКРУГА - ЮГРЫ "СУРГУТСКИЙ МНОГОПРОФИЛЬНЫЙ РЕАБИЛИТАЦИОННЫЙ ЦЕНТР ДЛЯ ИНВАЛИДОВ"</t>
+          <t>АКЦИОНЕРНОЕ ОБЩЕСТВО "ВОЛОГДАГОРТЕПЛОСЕТЬ"</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Поставка основных средств (проектор)</t>
+          <t>Поставка установки умягчения воды АКВАФЛОУ</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>49 666,67 ₽</t>
+          <t>2 111 815,33 ₽</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 17.11.2025</t>
+          <t>29.10.2025, 29.10.2025, 10.11.2025</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
+          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996843</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18953410</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>№ 32515385094</t>
+          <t>№ 32515350060</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "ВОДОКАНАЛ"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ КУЛЬТУРЫ "ДВОРЕЦ МЕТАЛЛУРГОВ"</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Работы по строительству наружных сетей водопровода путем строительства водопроводных сетей г. Мелеуз, Республики Башкортостан (протяженность L=2,6 км, ПЭ 110 мм)</t>
+          <t>Поставка полотна холстопрошивного</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>3 303 200,19 ₽</t>
+          <t>48 633,00 ₽</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 18.11.2025</t>
+          <t>29.10.2025, 29.10.2025, 06.11.2025</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -3895,108 +3907,108 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996823</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18952384</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>№ 32515385090</t>
+          <t>№ 32515350188</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ РЕСПУБЛИКИ БАШКОРТОСТАН СТОМАТОЛОГИЧЕСКАЯ ПОЛИКЛИНИКА ГОРОДА СТЕРЛИТАМАК</t>
+          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ ДОПОЛНИТЕЛЬНОГО ОБРАЗОВАНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "СПОРТИВНАЯ ШКОЛА ОЛИМПИЙСКОГО РЕЗЕРВА "ВИТЯЗЬ"</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Поставка стола-тумбы лабораторного</t>
+          <t>Оказание услуг по обслуживанию чаши бассейна и системы водоподготовки (оборотного водоснабжения) на 2026 год</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>252 000,00 ₽</t>
+          <t>492 000,00 ₽</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>29.10.2025, 29.10.2025, 06.11.2025</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996772</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18952286</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>№ 32515385089</t>
+          <t>№ 32515350147</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ ОБЩЕОБРАЗОВАТЕЛЬНОЕ УЧРЕЖДЕНИЕ "СРЕДНЯЯ ОБЩЕОБРАЗОВАТЕЛЬНАЯ ШКОЛА С. ОКУНЁВО"</t>
+          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ КУЛЬТУРЫ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКИЙ ОРДЕНА "ЗНАК ПОЧЕТА" ГОСУДАРСТВЕННЫЙ ДРАМАТИЧЕСКИЙ ТЕАТР"</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Поставка тепловой энергии</t>
+          <t>Оказание услуг по уборке и содержанию прилегающих территорий к зданию Автономного учреждения культуры Вологодской области «Вологодского ордена «Знак Почета» государственный драматический театр»</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>3 938 793,48 ₽</t>
+          <t>2 160 000,00 ₽</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>29.10.2025, 29.10.2025, 06.11.2025</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>223-ФЗ Закупка у единственного поставщика (подрядчика, исполнителя)</t>
+          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996813</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18952227</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>№ 32515385080</t>
+          <t>№ 32515350002</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ КУЛЬТУРЫ "ОРЕНБУРГСКАЯ ОБЛАСТНАЯ ФИЛАРМОНИЯ"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ КУЛЬТУРЫ "ДВОРЕЦ МЕТАЛЛУРГОВ"</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Проведение в рамках капитального ремонта работ по сохранению объекта культурного наследия регионального значения "Дом купца В.Н. Ладыгина" расположенного по адресу : г. Оренбург, ул. Пролетарская/ Володарского/ Советская, 39/10/52</t>
+          <t>Поставка бумаги санитарно -гигиенического назначения</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>148 810,00 ₽</t>
+          <t>116 246,50 ₽</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025</t>
+          <t>29.10.2025, 29.10.2025, 06.11.2025</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -4006,108 +4018,108 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996815</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18952119</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>№ 32515377583</t>
+          <t>№ 32515350015</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "ЛАНГЕПАССКИЕ КОММУНАЛЬНЫЕ СИСТЕМЫ"</t>
+          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ КУЛЬТУРЫ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКИЙ ОРДЕНА "ЗНАК ПОЧЕТА" ГОСУДАРСТВЕННЫЙ ДРАМАТИЧЕСКИЙ ТЕАТР"</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Оказание охранных услуг на объекте Заказчика</t>
+          <t>Оказание услуг по уборке помещений в здании АУК ВО «Вологодский драматический театр»</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>8 738 100,00 ₽</t>
+          <t>4 056 000,00 ₽</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>07.11.2025, 10.11.2025, 24.11.2025</t>
+          <t>29.10.2025, 29.10.2025, 06.11.2025</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Аукцион в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996811</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18952025</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>№ 32515371897</t>
+          <t>№ 32515349945</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ ГОРОДА НИЖНЕВАРТОВСКА "ДИРЕКЦИЯ СПОРТИВНЫХ СООРУЖЕНИЙ"</t>
+          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ ФИЗИЧЕСКОЙ КУЛЬТУРЫ И СПОРТА ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР СПОРТИВНОЙ ПОДГОТОВКИ"</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Приобретение арочного металлодетектора в 2025 году</t>
+          <t>Оказание услуг по дератизации, дезинсекции и дезинфекции</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>138 996,67 ₽</t>
+          <t>298 760,00 ₽</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>05.11.2025, 10.11.2025, 11.11.2025</t>
+          <t>29.10.2025, 29.10.2025, 10.11.2025</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>223-ФЗ Прочие</t>
+          <t>223-ФЗ Запрос котировок в электронной форме, участниками которого могут являться только субъекты малого и среднего предпринимательства</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18996818</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18951922</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>№ 32515381588</t>
+          <t>№ 32515349834</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ "АГИНСКАЯ ЦЕНТРАЛЬНАЯ РАЙОННАЯ БОЛЬНИЦА"</t>
+          <t>АВТОНОМНОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ОБЛАСТНОЙ ЦЕНТР МОЛОДЕЖНЫХ И ГРАЖДАНСКИХ ИНИЦИАТИВ "СОДРУЖЕСТВО"</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Поставка реагентов для анализатора "ALISEI Q.S."</t>
+          <t>Оказание услуг по организации проживания, предоставлению помещений для проведения областного слета студенческого актива «ОССА»</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>2 560 757,09 ₽</t>
+          <t>785 000,00 ₽</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 10.11.2025</t>
+          <t>29.10.2025, 29.10.2025, 07.11.2025</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -4117,34 +4129,34 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18994571</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18951631</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>№ 32515383605</t>
+          <t>№ 32515349712</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ ПРЕДПРИЯТИЕ РЕСПУБЛИКИ БУРЯТИЯ "БУРЯТ-ФАРМАЦИЯ"</t>
+          <t>МУНИЦИПАЛЬНОЕ АВТОНОМНОЕ УЧРЕЖДЕНИЕ КУЛЬТУРЫ "ДВОРЕЦ МЕТАЛЛУРГОВ"</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Поставка лекарственных препаратов</t>
+          <t>Поставка Бытовой химии</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>4 400 445,94 ₽</t>
+          <t>227 529,58 ₽</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>10.11.2025, 10.11.2025, 14.11.2025</t>
+          <t>29.10.2025, 29.10.2025, 06.11.2025</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -4154,7 +4166,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18995018</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/notice223/common-info.html?noticeInfoId=18951497</t>
         </is>
       </c>
     </row>

</xml_diff>